<commit_message>
Kleine aanpassingen testcase en aanpassen testdata
</commit_message>
<xml_diff>
--- a/test/testdata.xlsx
+++ b/test/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Blockathon_hyper42\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F85E5F-148F-4A5E-8A0C-5B1ED5983D8D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D5FF57-2A63-47C0-85AC-A7DA7C563415}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="428">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Fila</t>
   </si>
   <si>
-    <t>Fjällräven</t>
-  </si>
-  <si>
     <t>Fossil</t>
   </si>
   <si>
@@ -440,15 +437,9 @@
     <t>Bluemint</t>
   </si>
   <si>
-    <t>BOND NO. 9</t>
-  </si>
-  <si>
     <t>Breil</t>
   </si>
   <si>
-    <t>Bric's</t>
-  </si>
-  <si>
     <t>Bricktown World</t>
   </si>
   <si>
@@ -473,9 +464,6 @@
     <t>Bvlgari</t>
   </si>
   <si>
-    <t>C.P. Company</t>
-  </si>
-  <si>
     <t>Canada Goose</t>
   </si>
   <si>
@@ -494,18 +482,9 @@
     <t>CHANEL</t>
   </si>
   <si>
-    <t>Chasin'</t>
-  </si>
-  <si>
-    <t>Church's</t>
-  </si>
-  <si>
     <t>City Cufflinks</t>
   </si>
   <si>
-    <t>Claesen's</t>
-  </si>
-  <si>
     <t>Clarins</t>
   </si>
   <si>
@@ -581,9 +560,6 @@
     <t>DOIY</t>
   </si>
   <si>
-    <t>Drake's</t>
-  </si>
-  <si>
     <t>ellesse</t>
   </si>
   <si>
@@ -593,9 +569,6 @@
     <t>Essenza</t>
   </si>
   <si>
-    <t>Estée Lauder</t>
-  </si>
-  <si>
     <t>ETQ</t>
   </si>
   <si>
@@ -662,9 +635,6 @@
     <t>Happy Socks</t>
   </si>
   <si>
-    <t>HERMÈS</t>
-  </si>
-  <si>
     <t>Herschel Supply</t>
   </si>
   <si>
@@ -686,9 +656,6 @@
     <t>IZIPIZI</t>
   </si>
   <si>
-    <t>J.Crew</t>
-  </si>
-  <si>
     <t>Jaguar</t>
   </si>
   <si>
@@ -719,9 +686,6 @@
     <t>KENZO</t>
   </si>
   <si>
-    <t>Kiehl's</t>
-  </si>
-  <si>
     <t>Kikkerland</t>
   </si>
   <si>
@@ -737,9 +701,6 @@
     <t>Lancaster</t>
   </si>
   <si>
-    <t>Lancôme</t>
-  </si>
-  <si>
     <t>Larsson &amp; Jennings</t>
   </si>
   <si>
@@ -767,9 +728,6 @@
     <t>Maen</t>
   </si>
   <si>
-    <t>Maison Kitsuné</t>
-  </si>
-  <si>
     <t>Maison Margiela</t>
   </si>
   <si>
@@ -827,9 +785,6 @@
     <t>Moroccanoil</t>
   </si>
   <si>
-    <t>M·A·C</t>
-  </si>
-  <si>
     <t>Narciso Rodriguez</t>
   </si>
   <si>
@@ -845,9 +800,6 @@
     <t>Nikos</t>
   </si>
   <si>
-    <t>NN07</t>
-  </si>
-  <si>
     <t>Nobis</t>
   </si>
   <si>
@@ -950,9 +902,6 @@
     <t>RVLT Revolution</t>
   </si>
   <si>
-    <t>Samsøe &amp; Samsøe</t>
-  </si>
-  <si>
     <t>Sandqvist</t>
   </si>
   <si>
@@ -1058,9 +1007,6 @@
     <t>TOM FORD</t>
   </si>
   <si>
-    <t>Tumble 'n Dry</t>
-  </si>
-  <si>
     <t>Tumi</t>
   </si>
   <si>
@@ -1103,9 +1049,6 @@
     <t>Welter Shelter</t>
   </si>
   <si>
-    <t>Wood'd</t>
-  </si>
-  <si>
     <t>Y-3</t>
   </si>
   <si>
@@ -1133,9 +1076,6 @@
     <t>HoutBrox</t>
   </si>
   <si>
-    <t>Hunkemöller</t>
-  </si>
-  <si>
     <t>Mexx</t>
   </si>
   <si>
@@ -1338,6 +1278,39 @@
   </si>
   <si>
     <t>EnforcementDBUrl</t>
+  </si>
+  <si>
+    <t>Hunkemoller</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Tumble n Dry</t>
+  </si>
+  <si>
+    <t>Lancome</t>
+  </si>
+  <si>
+    <t>HERMES</t>
+  </si>
+  <si>
+    <t>Estee Lauder</t>
+  </si>
+  <si>
+    <t>Drake</t>
+  </si>
+  <si>
+    <t>Chasin</t>
+  </si>
+  <si>
+    <t>Churchs</t>
+  </si>
+  <si>
+    <t>Claesens</t>
+  </si>
+  <si>
+    <t>Brics</t>
   </si>
 </sst>
 </file>
@@ -1689,10 +1662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3382E85-A5EE-423B-83A5-84997E0C5C39}">
-  <dimension ref="A1:A354"/>
+  <dimension ref="A1:A345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="F375" sqref="F375"/>
+    <sheetView tabSelected="1" topLeftCell="A293" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1707,12 +1680,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
@@ -1722,7 +1695,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -1732,12 +1705,12 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -1747,27 +1720,27 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
@@ -1777,12 +1750,12 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
@@ -1792,17 +1765,17 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
@@ -1812,12 +1785,12 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
@@ -1827,522 +1800,522 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>427</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>424</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>154</v>
+        <v>425</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>156</v>
+        <v>426</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>158</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>22</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>23</v>
+        <v>174</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>24</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>182</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>183</v>
+        <v>423</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>184</v>
+        <v>27</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>28</v>
+        <v>178</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>186</v>
+        <v>422</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>187</v>
+        <v>29</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>189</v>
+        <v>31</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>30</v>
+        <v>181</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>32</v>
+        <v>183</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>192</v>
+        <v>33</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>33</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>193</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>34</v>
+        <v>186</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>35</v>
+        <v>188</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>202</v>
+        <v>35</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>203</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>36</v>
+        <v>196</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
@@ -2352,187 +2325,187 @@
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>2</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>38</v>
+        <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>206</v>
+        <v>38</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>208</v>
+        <v>39</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>209</v>
+        <v>40</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>210</v>
+        <v>421</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>41</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>42</v>
+        <v>203</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>212</v>
+        <v>43</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>213</v>
+        <v>44</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>44</v>
+        <v>206</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>215</v>
+        <v>45</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>216</v>
+        <v>46</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>46</v>
+        <v>209</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>47</v>
+        <v>210</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>218</v>
+        <v>48</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>219</v>
+        <v>49</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>49</v>
+        <v>213</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>50</v>
+        <v>214</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>225</v>
+        <v>50</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>226</v>
+        <v>51</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>51</v>
+        <v>220</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
@@ -2542,932 +2515,887 @@
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>230</v>
+        <v>53</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>53</v>
+        <v>420</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>233</v>
+        <v>54</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>54</v>
+        <v>224</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>235</v>
+        <v>55</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>237</v>
+        <v>56</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>56</v>
+        <v>229</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>57</v>
+        <v>232</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>242</v>
+        <v>57</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>244</v>
+        <v>58</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>58</v>
+        <v>238</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>59</v>
+        <v>240</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>251</v>
+        <v>59</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>60</v>
+        <v>248</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>262</v>
+        <v>60</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>264</v>
+        <v>61</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>265</v>
+        <v>62</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>267</v>
+        <v>1</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>62</v>
+        <v>258</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>63</v>
+        <v>259</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>271</v>
+        <v>65</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>64</v>
+        <v>261</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>275</v>
+        <v>66</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>280</v>
+        <v>69</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>67</v>
+        <v>269</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>68</v>
+        <v>271</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>282</v>
+        <v>72</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>283</v>
+        <v>71</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>70</v>
+        <v>273</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>72</v>
+        <v>277</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>289</v>
+        <v>75</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>292</v>
+        <v>76</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>294</v>
+        <v>79</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>78</v>
+        <v>284</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>79</v>
+        <v>285</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>80</v>
+        <v>287</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>81</v>
+        <v>288</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>298</v>
+        <v>83</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>82</v>
+        <v>290</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>300</v>
+        <v>84</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>301</v>
+        <v>85</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>302</v>
+        <v>86</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>85</v>
+        <v>295</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>86</v>
+        <v>296</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>87</v>
+        <v>297</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>88</v>
+        <v>301</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
-        <v>326</v>
+        <v>6</v>
       </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
-        <v>327</v>
+        <v>89</v>
       </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
-        <v>331</v>
+        <v>91</v>
       </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
-        <v>334</v>
+        <v>92</v>
       </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>6</v>
+        <v>323</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
-        <v>337</v>
+        <v>94</v>
       </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>338</v>
+        <v>419</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>93</v>
+        <v>327</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>341</v>
+        <v>97</v>
       </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
-        <v>342</v>
+        <v>98</v>
       </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>95</v>
+        <v>329</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>96</v>
+        <v>330</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>98</v>
+        <v>335</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>99</v>
+        <v>336</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
-        <v>350</v>
+        <v>100</v>
       </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>351</v>
+        <v>418</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>100</v>
+        <v>341</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A342" t="s">
-        <v>355</v>
+        <v>101</v>
       </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
-        <v>356</v>
+        <v>102</v>
       </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>357</v>
+        <v>344</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A346" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A347" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A348" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A349" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A350" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A351" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A352" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A353" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A354" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -3479,8 +3407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBAF63-11C6-4E85-926A-7576D04BFACD}">
   <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3495,102 +3423,102 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>383</v>
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>376</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>389</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>390</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>391</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>392</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>393</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>394</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
@@ -3600,107 +3528,107 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>395</v>
+        <v>375</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>368</v>
+        <v>417</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>396</v>
+        <v>376</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>397</v>
+        <v>377</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>398</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>399</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>400</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>404</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>405</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>369</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>406</v>
+        <v>386</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>407</v>
+        <v>387</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
@@ -3710,82 +3638,82 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>410</v>
+        <v>390</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>371</v>
+        <v>351</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>412</v>
+        <v>392</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>417</v>
+        <v>397</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>418</v>
+        <v>398</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>419</v>
+        <v>399</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>420</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>421</v>
+        <v>401</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
@@ -3795,42 +3723,42 @@
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>423</v>
+        <v>403</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>424</v>
+        <v>404</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>372</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>373</v>
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>425</v>
+        <v>405</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>426</v>
+        <v>406</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>427</v>
+        <v>407</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
@@ -3840,42 +3768,42 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>428</v>
+        <v>408</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>429</v>
+        <v>409</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>430</v>
+        <v>410</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>374</v>
+        <v>354</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>431</v>
+        <v>411</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>375</v>
+        <v>355</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>379</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
@@ -3885,7 +3813,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>432</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -3914,16 +3842,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>433</v>
+        <v>413</v>
       </c>
       <c r="B1" t="s">
-        <v>434</v>
+        <v>414</v>
       </c>
       <c r="C1" t="s">
-        <v>435</v>
+        <v>415</v>
       </c>
       <c r="D1" t="s">
-        <v>436</v>
+        <v>416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testdata douane plus, testcase opvoeren bulk douane.
</commit_message>
<xml_diff>
--- a/test/testdata.xlsx
+++ b/test/testdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Blockathon_hyper42\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35344602-F2FF-4F5E-936F-CB5F4801D38A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969868E2-8BBB-4D11-9F96-5639FF20F294}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Manufacturer" sheetId="1" r:id="rId1"/>
     <sheet name="Orderer" sheetId="2" r:id="rId2"/>
     <sheet name="Product" sheetId="3" r:id="rId3"/>
+    <sheet name="Douane" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="439">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -722,9 +723,6 @@
     <t>Maison Margiela</t>
   </si>
   <si>
-    <t>Marc O'Polo</t>
-  </si>
-  <si>
     <t>Mason Garments</t>
   </si>
   <si>
@@ -1190,9 +1188,6 @@
     <t>PME Legend</t>
   </si>
   <si>
-    <t>Polarn O. Pyret</t>
-  </si>
-  <si>
     <t>Promiss</t>
   </si>
   <si>
@@ -1311,6 +1306,45 @@
   </si>
   <si>
     <t>eyes more</t>
+  </si>
+  <si>
+    <t>Polarn O Pyret</t>
+  </si>
+  <si>
+    <t>Marc O Polo</t>
+  </si>
+  <si>
+    <t>Douane</t>
+  </si>
+  <si>
+    <t>Douane Amsterdam</t>
+  </si>
+  <si>
+    <t>Douane Rotterdam</t>
+  </si>
+  <si>
+    <t>Douane Antwerpen</t>
+  </si>
+  <si>
+    <t>Douane Brussel</t>
+  </si>
+  <si>
+    <t>Douane New York</t>
+  </si>
+  <si>
+    <t>Douane China</t>
+  </si>
+  <si>
+    <t>Douane Suriname</t>
+  </si>
+  <si>
+    <t>Douane India</t>
+  </si>
+  <si>
+    <t>Douane Frankrijk</t>
+  </si>
+  <si>
+    <t>Douane Spanje</t>
   </si>
 </sst>
 </file>
@@ -1664,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3382E85-A5EE-423B-83A5-84997E0C5C39}">
   <dimension ref="A1:A345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A278" sqref="A278"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A187" sqref="A187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,7 +1899,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -1890,7 +1924,7 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
@@ -1975,12 +2009,12 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
@@ -1990,7 +2024,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
@@ -2035,7 +2069,7 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
@@ -2150,7 +2184,7 @@
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
@@ -2185,7 +2219,7 @@
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
@@ -2370,7 +2404,7 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
@@ -2535,7 +2569,7 @@
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
@@ -2570,7 +2604,7 @@
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
@@ -2610,7 +2644,7 @@
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>231</v>
+        <v>427</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
@@ -2620,42 +2654,42 @@
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
@@ -2665,57 +2699,57 @@
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
@@ -2725,7 +2759,7 @@
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
@@ -2740,7 +2774,7 @@
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
@@ -2750,7 +2784,7 @@
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
@@ -2760,22 +2794,22 @@
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.3">
@@ -2790,22 +2824,22 @@
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.3">
@@ -2815,7 +2849,7 @@
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.3">
@@ -2830,17 +2864,17 @@
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.3">
@@ -2850,17 +2884,17 @@
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.3">
@@ -2880,27 +2914,27 @@
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.3">
@@ -2915,12 +2949,12 @@
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.3">
@@ -2930,12 +2964,12 @@
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.3">
@@ -2955,7 +2989,7 @@
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.3">
@@ -2970,12 +3004,12 @@
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.3">
@@ -2985,27 +3019,27 @@
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.3">
@@ -3015,12 +3049,12 @@
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.3">
@@ -3040,12 +3074,12 @@
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.3">
@@ -3055,127 +3089,127 @@
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.3">
@@ -3190,17 +3224,17 @@
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.3">
@@ -3210,12 +3244,12 @@
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.3">
@@ -3225,7 +3259,7 @@
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.3">
@@ -3235,12 +3269,12 @@
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.3">
@@ -3255,22 +3289,22 @@
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.3">
@@ -3290,32 +3324,32 @@
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.3">
@@ -3325,27 +3359,27 @@
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.3">
@@ -3355,27 +3389,27 @@
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A338" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A340" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.3">
@@ -3390,12 +3424,12 @@
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A344" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3407,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FBAF63-11C6-4E85-926A-7576D04BFACD}">
   <dimension ref="A1:A80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3428,92 +3462,92 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
@@ -3528,17 +3562,17 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
@@ -3548,87 +3582,87 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
@@ -3638,32 +3672,32 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>387</v>
+        <v>426</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
@@ -3673,42 +3707,42 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
@@ -3728,37 +3762,37 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
@@ -3768,42 +3802,42 @@
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
@@ -3813,7 +3847,7 @@
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -3842,16 +3876,89 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C1" t="s">
         <v>407</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>408</v>
       </c>
-      <c r="C1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D1" t="s">
-        <v>410</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6C8FFF-B55A-4223-8A3A-B7DB0DBD20CE}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testdata voor Transporter + Testcase opvoeren bulk transporter
</commit_message>
<xml_diff>
--- a/test/testdata.xlsx
+++ b/test/testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Blockathon_hyper42\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969868E2-8BBB-4D11-9F96-5639FF20F294}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4D63B1-6804-41C2-9FA3-A85D1FF405ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="4" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Manufacturer" sheetId="1" r:id="rId1"/>
     <sheet name="Orderer" sheetId="2" r:id="rId2"/>
-    <sheet name="Product" sheetId="3" r:id="rId3"/>
-    <sheet name="Douane" sheetId="4" r:id="rId4"/>
+    <sheet name="Douane" sheetId="4" r:id="rId3"/>
+    <sheet name="Product" sheetId="3" r:id="rId4"/>
+    <sheet name="Transporter" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="521">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -1245,18 +1246,12 @@
     <t>Zinzi</t>
   </si>
   <si>
-    <t>ProductID</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Value</t>
   </si>
   <si>
-    <t>EnforcementDBUrl</t>
-  </si>
-  <si>
     <t>Hunkemoller</t>
   </si>
   <si>
@@ -1345,6 +1340,258 @@
   </si>
   <si>
     <t>Douane Spanje</t>
+  </si>
+  <si>
+    <t>Afritsbroek</t>
+  </si>
+  <si>
+    <t>Badpak</t>
+  </si>
+  <si>
+    <t>Bandana</t>
+  </si>
+  <si>
+    <t>Bergschoenen</t>
+  </si>
+  <si>
+    <t>BHs</t>
+  </si>
+  <si>
+    <t>Bikini</t>
+  </si>
+  <si>
+    <t>Bikinibroekje</t>
+  </si>
+  <si>
+    <t>Blouses</t>
+  </si>
+  <si>
+    <t>Bodywarmer</t>
+  </si>
+  <si>
+    <t>Boxershorts</t>
+  </si>
+  <si>
+    <t>Broeken</t>
+  </si>
+  <si>
+    <t>Broekriem</t>
+  </si>
+  <si>
+    <t>Campingsmoking</t>
+  </si>
+  <si>
+    <t>Driekwart broeken</t>
+  </si>
+  <si>
+    <t>Fleece-trui</t>
+  </si>
+  <si>
+    <t>Geurvreters</t>
+  </si>
+  <si>
+    <t>Haarband</t>
+  </si>
+  <si>
+    <t>Handschoenen</t>
+  </si>
+  <si>
+    <t>Hemden</t>
+  </si>
+  <si>
+    <t>Hoed</t>
+  </si>
+  <si>
+    <t>Jas</t>
+  </si>
+  <si>
+    <t>Joggingpak</t>
+  </si>
+  <si>
+    <t>Jurken</t>
+  </si>
+  <si>
+    <t>Korte broeken</t>
+  </si>
+  <si>
+    <t>Laarzen</t>
+  </si>
+  <si>
+    <t>Lange broeken</t>
+  </si>
+  <si>
+    <t>Legging</t>
+  </si>
+  <si>
+    <t>Lingerie</t>
+  </si>
+  <si>
+    <t>Moonboots</t>
+  </si>
+  <si>
+    <t>Muts</t>
+  </si>
+  <si>
+    <t>Nette schoenen</t>
+  </si>
+  <si>
+    <t>Onderbroeken</t>
+  </si>
+  <si>
+    <t>Overhemden</t>
+  </si>
+  <si>
+    <t>Panties</t>
+  </si>
+  <si>
+    <t>Pantoffels</t>
+  </si>
+  <si>
+    <t>Pareo</t>
+  </si>
+  <si>
+    <t>Pet</t>
+  </si>
+  <si>
+    <t>Poncho</t>
+  </si>
+  <si>
+    <t>Pyjama</t>
+  </si>
+  <si>
+    <t>Regenjack</t>
+  </si>
+  <si>
+    <t>Regenpak</t>
+  </si>
+  <si>
+    <t>Rokken</t>
+  </si>
+  <si>
+    <t>Sandalen</t>
+  </si>
+  <si>
+    <t>Sarong</t>
+  </si>
+  <si>
+    <t>Schoenen</t>
+  </si>
+  <si>
+    <t>Shirts</t>
+  </si>
+  <si>
+    <t>Sjaal</t>
+  </si>
+  <si>
+    <t>Skihandschoenen</t>
+  </si>
+  <si>
+    <t>Skipak</t>
+  </si>
+  <si>
+    <t>Skischoenen</t>
+  </si>
+  <si>
+    <t>Skisokken</t>
+  </si>
+  <si>
+    <t>Slippers</t>
+  </si>
+  <si>
+    <t>Slips</t>
+  </si>
+  <si>
+    <t>Sloffen</t>
+  </si>
+  <si>
+    <t>Sokken</t>
+  </si>
+  <si>
+    <t>Spijkerjack</t>
+  </si>
+  <si>
+    <t>Sportschoenen</t>
+  </si>
+  <si>
+    <t>Stringtanga</t>
+  </si>
+  <si>
+    <t>Stropdas</t>
+  </si>
+  <si>
+    <t>Sweaters</t>
+  </si>
+  <si>
+    <t>T-shirts</t>
+  </si>
+  <si>
+    <t>Thermo-kleding</t>
+  </si>
+  <si>
+    <t>Trainingspak</t>
+  </si>
+  <si>
+    <t>Truien</t>
+  </si>
+  <si>
+    <t>Uitgaanskleding</t>
+  </si>
+  <si>
+    <t>Vest</t>
+  </si>
+  <si>
+    <t>Veters</t>
+  </si>
+  <si>
+    <t>Wandelschoenen</t>
+  </si>
+  <si>
+    <t>Waterschoentjes</t>
+  </si>
+  <si>
+    <t>Windjack</t>
+  </si>
+  <si>
+    <t>Zeilpak</t>
+  </si>
+  <si>
+    <t>Zonnebril</t>
+  </si>
+  <si>
+    <t>Zwembroek</t>
+  </si>
+  <si>
+    <t>Transporter</t>
+  </si>
+  <si>
+    <t>TNT</t>
+  </si>
+  <si>
+    <t>DHL</t>
+  </si>
+  <si>
+    <t>PostNL</t>
+  </si>
+  <si>
+    <t>UPS</t>
+  </si>
+  <si>
+    <t>FedEx</t>
+  </si>
+  <si>
+    <t>Panalpina</t>
+  </si>
+  <si>
+    <t>DSV</t>
+  </si>
+  <si>
+    <t>CEVA Logistics</t>
+  </si>
+  <si>
+    <t>Nippon Express</t>
+  </si>
+  <si>
+    <t>Maersk</t>
   </si>
 </sst>
 </file>
@@ -1899,7 +2146,7 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
@@ -1924,7 +2171,7 @@
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
@@ -2009,12 +2256,12 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
@@ -2024,7 +2271,7 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
@@ -2069,7 +2316,7 @@
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
@@ -2184,7 +2431,7 @@
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
@@ -2219,7 +2466,7 @@
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
@@ -2404,7 +2651,7 @@
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
@@ -2569,7 +2816,7 @@
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
@@ -2604,7 +2851,7 @@
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
@@ -2644,7 +2891,7 @@
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
@@ -3094,7 +3341,7 @@
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.3">
@@ -3289,7 +3536,7 @@
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.3">
@@ -3389,7 +3636,7 @@
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.3">
@@ -3472,7 +3719,7 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
@@ -3537,7 +3784,7 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
@@ -3572,7 +3819,7 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
@@ -3692,7 +3939,7 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
@@ -3859,45 +4106,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C3947-283C-45EE-B2FB-975473C10A44}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>405</v>
-      </c>
-      <c r="B1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D1" t="s">
-        <v>408</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6C8FFF-B55A-4223-8A3A-B7DB0DBD20CE}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -3908,57 +4120,738 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C3947-283C-45EE-B2FB-975473C10A44}">
+  <dimension ref="A1:B74"/>
+  <sheetViews>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>405</v>
+      </c>
+      <c r="B1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>438</v>
+      </c>
+      <c r="B3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>442</v>
+      </c>
+      <c r="B7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>443</v>
+      </c>
+      <c r="B8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>444</v>
+      </c>
+      <c r="B9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>445</v>
+      </c>
+      <c r="B10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>446</v>
+      </c>
+      <c r="B11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>447</v>
+      </c>
+      <c r="B12">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>448</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>449</v>
+      </c>
+      <c r="B14">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>450</v>
+      </c>
+      <c r="B15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>451</v>
+      </c>
+      <c r="B16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>452</v>
+      </c>
+      <c r="B17">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>453</v>
+      </c>
+      <c r="B18">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>454</v>
+      </c>
+      <c r="B19">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>455</v>
+      </c>
+      <c r="B20">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>456</v>
+      </c>
+      <c r="B21">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>457</v>
+      </c>
+      <c r="B22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>458</v>
+      </c>
+      <c r="B23">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>459</v>
+      </c>
+      <c r="B24">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>460</v>
+      </c>
+      <c r="B25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>461</v>
+      </c>
+      <c r="B26">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B27">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>463</v>
+      </c>
+      <c r="B28">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>464</v>
+      </c>
+      <c r="B29">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>465</v>
+      </c>
+      <c r="B30">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>466</v>
+      </c>
+      <c r="B31">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>467</v>
+      </c>
+      <c r="B32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>468</v>
+      </c>
+      <c r="B33">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>469</v>
+      </c>
+      <c r="B34">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>470</v>
+      </c>
+      <c r="B35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>471</v>
+      </c>
+      <c r="B36">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>472</v>
+      </c>
+      <c r="B37">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>473</v>
+      </c>
+      <c r="B38">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>474</v>
+      </c>
+      <c r="B39">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>475</v>
+      </c>
+      <c r="B40">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>476</v>
+      </c>
+      <c r="B41">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>477</v>
+      </c>
+      <c r="B42">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>478</v>
+      </c>
+      <c r="B43">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>479</v>
+      </c>
+      <c r="B44">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>480</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>481</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>482</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>483</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>484</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>485</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>486</v>
+      </c>
+      <c r="B51">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>487</v>
+      </c>
+      <c r="B52">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>488</v>
+      </c>
+      <c r="B53">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>489</v>
+      </c>
+      <c r="B54">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>490</v>
+      </c>
+      <c r="B55">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>491</v>
+      </c>
+      <c r="B56">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>492</v>
+      </c>
+      <c r="B57">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>493</v>
+      </c>
+      <c r="B58">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>494</v>
+      </c>
+      <c r="B59">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>495</v>
+      </c>
+      <c r="B60">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>496</v>
+      </c>
+      <c r="B61">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>497</v>
+      </c>
+      <c r="B62">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>498</v>
+      </c>
+      <c r="B63">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>499</v>
+      </c>
+      <c r="B64">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>500</v>
+      </c>
+      <c r="B65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>501</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>502</v>
+      </c>
+      <c r="B67">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>503</v>
+      </c>
+      <c r="B68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>504</v>
+      </c>
+      <c r="B69">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>505</v>
+      </c>
+      <c r="B70">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>506</v>
+      </c>
+      <c r="B71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>507</v>
+      </c>
+      <c r="B72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>508</v>
+      </c>
+      <c r="B73">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>509</v>
+      </c>
+      <c r="B74">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121834CB-7DB5-4DE5-9063-174FC24C506B}">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testdata aangepast voor product + testcase aangepast
</commit_message>
<xml_diff>
--- a/test/testdata.xlsx
+++ b/test/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Blockathon_hyper42\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068F0211-39C6-4E12-AAB1-249C40A77190}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DCA278-406F-48F4-BF30-4E6AC9185B47}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="921">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="1069">
   <si>
     <t>Nike</t>
   </si>
@@ -2792,16 +2792,468 @@
   </si>
   <si>
     <t>Creator</t>
+  </si>
+  <si>
+    <t>ProductID</t>
+  </si>
+  <si>
+    <t>ProductID0001</t>
+  </si>
+  <si>
+    <t>ProductID0002</t>
+  </si>
+  <si>
+    <t>ProductID0003</t>
+  </si>
+  <si>
+    <t>ProductID0004</t>
+  </si>
+  <si>
+    <t>ProductID0005</t>
+  </si>
+  <si>
+    <t>ProductID0006</t>
+  </si>
+  <si>
+    <t>ProductID0007</t>
+  </si>
+  <si>
+    <t>ProductID0008</t>
+  </si>
+  <si>
+    <t>ProductID0009</t>
+  </si>
+  <si>
+    <t>ProductID0010</t>
+  </si>
+  <si>
+    <t>ProductID0011</t>
+  </si>
+  <si>
+    <t>ProductID0012</t>
+  </si>
+  <si>
+    <t>ProductID0013</t>
+  </si>
+  <si>
+    <t>ProductID0014</t>
+  </si>
+  <si>
+    <t>ProductID0015</t>
+  </si>
+  <si>
+    <t>ProductID0016</t>
+  </si>
+  <si>
+    <t>ProductID0017</t>
+  </si>
+  <si>
+    <t>ProductID0018</t>
+  </si>
+  <si>
+    <t>ProductID0019</t>
+  </si>
+  <si>
+    <t>ProductID0020</t>
+  </si>
+  <si>
+    <t>ProductID0021</t>
+  </si>
+  <si>
+    <t>ProductID0022</t>
+  </si>
+  <si>
+    <t>ProductID0023</t>
+  </si>
+  <si>
+    <t>ProductID0024</t>
+  </si>
+  <si>
+    <t>ProductID0025</t>
+  </si>
+  <si>
+    <t>ProductID0026</t>
+  </si>
+  <si>
+    <t>ProductID0027</t>
+  </si>
+  <si>
+    <t>ProductID0028</t>
+  </si>
+  <si>
+    <t>ProductID0029</t>
+  </si>
+  <si>
+    <t>ProductID0030</t>
+  </si>
+  <si>
+    <t>ProductID0031</t>
+  </si>
+  <si>
+    <t>ProductID0032</t>
+  </si>
+  <si>
+    <t>ProductID0033</t>
+  </si>
+  <si>
+    <t>ProductID0034</t>
+  </si>
+  <si>
+    <t>ProductID0035</t>
+  </si>
+  <si>
+    <t>ProductID0036</t>
+  </si>
+  <si>
+    <t>ProductID0037</t>
+  </si>
+  <si>
+    <t>ProductID0038</t>
+  </si>
+  <si>
+    <t>ProductID0039</t>
+  </si>
+  <si>
+    <t>ProductID0040</t>
+  </si>
+  <si>
+    <t>ProductID0041</t>
+  </si>
+  <si>
+    <t>ProductID0042</t>
+  </si>
+  <si>
+    <t>ProductID0043</t>
+  </si>
+  <si>
+    <t>ProductID0044</t>
+  </si>
+  <si>
+    <t>ProductID0045</t>
+  </si>
+  <si>
+    <t>ProductID0046</t>
+  </si>
+  <si>
+    <t>ProductID0047</t>
+  </si>
+  <si>
+    <t>ProductID0048</t>
+  </si>
+  <si>
+    <t>ProductID0049</t>
+  </si>
+  <si>
+    <t>ProductID0050</t>
+  </si>
+  <si>
+    <t>ProductID0051</t>
+  </si>
+  <si>
+    <t>ProductID0052</t>
+  </si>
+  <si>
+    <t>ProductID0053</t>
+  </si>
+  <si>
+    <t>ProductID0054</t>
+  </si>
+  <si>
+    <t>ProductID0055</t>
+  </si>
+  <si>
+    <t>ProductID0056</t>
+  </si>
+  <si>
+    <t>ProductID0057</t>
+  </si>
+  <si>
+    <t>ProductID0058</t>
+  </si>
+  <si>
+    <t>ProductID0059</t>
+  </si>
+  <si>
+    <t>ProductID0060</t>
+  </si>
+  <si>
+    <t>ProductID0061</t>
+  </si>
+  <si>
+    <t>ProductID0062</t>
+  </si>
+  <si>
+    <t>ProductID0063</t>
+  </si>
+  <si>
+    <t>ProductID0064</t>
+  </si>
+  <si>
+    <t>ProductID0065</t>
+  </si>
+  <si>
+    <t>ProductID0066</t>
+  </si>
+  <si>
+    <t>ProductID0067</t>
+  </si>
+  <si>
+    <t>ProductID0068</t>
+  </si>
+  <si>
+    <t>ProductID0069</t>
+  </si>
+  <si>
+    <t>ProductID0070</t>
+  </si>
+  <si>
+    <t>ProductID0071</t>
+  </si>
+  <si>
+    <t>ProductID0072</t>
+  </si>
+  <si>
+    <t>ProductID0073</t>
+  </si>
+  <si>
+    <t>EnforcementDBUrl</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0001</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0002</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0003</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0004</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0005</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0006</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0007</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0008</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0009</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0010</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0011</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0012</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0013</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0014</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0015</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0016</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0017</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0018</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0019</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0020</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0021</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0022</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0023</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0024</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0025</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0026</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0027</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0028</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0029</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0030</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0031</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0032</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0033</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0034</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0035</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0036</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0037</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0038</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0039</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0040</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0041</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0042</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0043</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0044</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0045</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0046</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0047</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0048</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0049</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0050</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0051</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0052</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0053</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0054</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0055</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0056</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0057</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0058</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0059</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0060</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0061</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0062</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0063</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0064</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0065</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0066</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0067</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0068</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0069</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0070</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0071</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0072</t>
+  </si>
+  <si>
+    <t>https://euipo.europa.eu/ohimportal/nl/databases/ProductID0073</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2824,13 +3276,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3145,8 +3600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3382E85-A5EE-423B-83A5-84997E0C5C39}">
   <dimension ref="A1:B324"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D318" sqref="D318"/>
+    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6521,614 +6976,1283 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C3947-283C-45EE-B2FB-975473C10A44}">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="60" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B1" t="s">
         <v>383</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>384</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>995</v>
+      </c>
+      <c r="E1" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>922</v>
+      </c>
+      <c r="B2" t="s">
         <v>412</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="E2" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>923</v>
+      </c>
+      <c r="B3" t="s">
         <v>413</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="E3" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>924</v>
+      </c>
+      <c r="B4" t="s">
         <v>414</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="E4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>925</v>
+      </c>
+      <c r="B5" t="s">
         <v>415</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="E5" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>926</v>
+      </c>
+      <c r="B6" t="s">
         <v>416</v>
       </c>
-      <c r="B6">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>927</v>
+      </c>
+      <c r="B7" t="s">
         <v>417</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E7" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>928</v>
+      </c>
+      <c r="B8" t="s">
         <v>418</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E8" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>929</v>
+      </c>
+      <c r="B9" t="s">
         <v>419</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E9" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>930</v>
+      </c>
+      <c r="B10" t="s">
         <v>420</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E10" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>931</v>
+      </c>
+      <c r="B11" t="s">
         <v>421</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E11" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>932</v>
+      </c>
+      <c r="B12" t="s">
         <v>422</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E12" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>933</v>
+      </c>
+      <c r="B13" t="s">
         <v>423</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="E13" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>934</v>
+      </c>
+      <c r="B14" t="s">
         <v>424</v>
       </c>
-      <c r="B14">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E14" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>935</v>
+      </c>
+      <c r="B15" t="s">
         <v>425</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="E15" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>936</v>
+      </c>
+      <c r="B16" t="s">
         <v>426</v>
       </c>
-      <c r="B16">
+      <c r="C16">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D16" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="E16" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>937</v>
+      </c>
+      <c r="B17" t="s">
         <v>427</v>
       </c>
-      <c r="B17">
+      <c r="C17">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D17" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="E17" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>938</v>
+      </c>
+      <c r="B18" t="s">
         <v>428</v>
       </c>
-      <c r="B18">
+      <c r="C18">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="E18" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>939</v>
+      </c>
+      <c r="B19" t="s">
         <v>429</v>
       </c>
-      <c r="B19">
+      <c r="C19">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="E19" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>940</v>
+      </c>
+      <c r="B20" t="s">
         <v>430</v>
       </c>
-      <c r="B20">
+      <c r="C20">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D20" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E20" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>941</v>
+      </c>
+      <c r="B21" t="s">
         <v>431</v>
       </c>
-      <c r="B21">
+      <c r="C21">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D21" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="E21" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>942</v>
+      </c>
+      <c r="B22" t="s">
         <v>432</v>
       </c>
-      <c r="B22">
+      <c r="C22">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E22" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>943</v>
+      </c>
+      <c r="B23" t="s">
         <v>433</v>
       </c>
-      <c r="B23">
+      <c r="C23">
         <v>66</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D23" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="E23" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>944</v>
+      </c>
+      <c r="B24" t="s">
         <v>434</v>
       </c>
-      <c r="B24">
+      <c r="C24">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D24" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E24" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>945</v>
+      </c>
+      <c r="B25" t="s">
         <v>435</v>
       </c>
-      <c r="B25">
+      <c r="C25">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D25" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E25" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>946</v>
+      </c>
+      <c r="B26" t="s">
         <v>436</v>
       </c>
-      <c r="B26">
+      <c r="C26">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D26" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E26" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>947</v>
+      </c>
+      <c r="B27" t="s">
         <v>437</v>
       </c>
-      <c r="B27">
+      <c r="C27">
         <v>72</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D27" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="E27" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>948</v>
+      </c>
+      <c r="B28" t="s">
         <v>438</v>
       </c>
-      <c r="B28">
+      <c r="C28">
         <v>74</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D28" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E28" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>949</v>
+      </c>
+      <c r="B29" t="s">
         <v>439</v>
       </c>
-      <c r="B29">
+      <c r="C29">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="E29" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>950</v>
+      </c>
+      <c r="B30" t="s">
         <v>440</v>
       </c>
-      <c r="B30">
+      <c r="C30">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="E30" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>951</v>
+      </c>
+      <c r="B31" t="s">
         <v>441</v>
       </c>
-      <c r="B31">
+      <c r="C31">
         <v>79</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>1025</v>
+      </c>
+      <c r="E31" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>952</v>
+      </c>
+      <c r="B32" t="s">
         <v>442</v>
       </c>
-      <c r="B32">
+      <c r="C32">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="E32" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>953</v>
+      </c>
+      <c r="B33" t="s">
         <v>443</v>
       </c>
-      <c r="B33">
+      <c r="C33">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33" s="1" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E33" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>954</v>
+      </c>
+      <c r="B34" t="s">
         <v>444</v>
       </c>
-      <c r="B34">
+      <c r="C34">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D34" s="1" t="s">
+        <v>1028</v>
+      </c>
+      <c r="E34" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>955</v>
+      </c>
+      <c r="B35" t="s">
         <v>445</v>
       </c>
-      <c r="B35">
+      <c r="C35">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="E35" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>956</v>
+      </c>
+      <c r="B36" t="s">
         <v>446</v>
       </c>
-      <c r="B36">
+      <c r="C36">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D36" s="1" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E36" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>957</v>
+      </c>
+      <c r="B37" t="s">
         <v>447</v>
       </c>
-      <c r="B37">
+      <c r="C37">
         <v>88</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D37" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E37" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>958</v>
+      </c>
+      <c r="B38" t="s">
         <v>448</v>
       </c>
-      <c r="B38">
+      <c r="C38">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D38" s="1" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E38" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>959</v>
+      </c>
+      <c r="B39" t="s">
         <v>449</v>
       </c>
-      <c r="B39">
+      <c r="C39">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D39" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="E39" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>960</v>
+      </c>
+      <c r="B40" t="s">
         <v>450</v>
       </c>
-      <c r="B40">
+      <c r="C40">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D40" s="1" t="s">
+        <v>1034</v>
+      </c>
+      <c r="E40" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>961</v>
+      </c>
+      <c r="B41" t="s">
         <v>451</v>
       </c>
-      <c r="B41">
+      <c r="C41">
         <v>95</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D41" s="1" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E41" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>962</v>
+      </c>
+      <c r="B42" t="s">
         <v>452</v>
       </c>
-      <c r="B42">
+      <c r="C42">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D42" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="E42" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>963</v>
+      </c>
+      <c r="B43" t="s">
         <v>453</v>
       </c>
-      <c r="B43">
+      <c r="C43">
         <v>98</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D43" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E43" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>964</v>
+      </c>
+      <c r="B44" t="s">
         <v>454</v>
       </c>
-      <c r="B44">
+      <c r="C44">
         <v>99</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D44" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E44" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>965</v>
+      </c>
+      <c r="B45" t="s">
         <v>455</v>
       </c>
-      <c r="B45">
+      <c r="C45">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D45" s="1" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E45" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>966</v>
+      </c>
+      <c r="B46" t="s">
         <v>456</v>
       </c>
-      <c r="B46">
+      <c r="C46">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D46" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E46" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>967</v>
+      </c>
+      <c r="B47" t="s">
         <v>457</v>
       </c>
-      <c r="B47">
+      <c r="C47">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D47" s="1" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E47" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>968</v>
+      </c>
+      <c r="B48" t="s">
         <v>458</v>
       </c>
-      <c r="B48">
+      <c r="C48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D48" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="E48" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>969</v>
+      </c>
+      <c r="B49" t="s">
         <v>459</v>
       </c>
-      <c r="B49">
+      <c r="C49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D49" s="1" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E49" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>970</v>
+      </c>
+      <c r="B50" t="s">
         <v>460</v>
       </c>
-      <c r="B50">
+      <c r="C50">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D50" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E50" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>971</v>
+      </c>
+      <c r="B51" t="s">
         <v>461</v>
       </c>
-      <c r="B51">
+      <c r="C51">
         <v>11</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E51" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>972</v>
+      </c>
+      <c r="B52" t="s">
         <v>462</v>
       </c>
-      <c r="B52">
+      <c r="C52">
         <v>13</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D52" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E52" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>973</v>
+      </c>
+      <c r="B53" t="s">
         <v>463</v>
       </c>
-      <c r="B53">
+      <c r="C53">
         <v>11</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D53" s="1" t="s">
+        <v>1047</v>
+      </c>
+      <c r="E53" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>974</v>
+      </c>
+      <c r="B54" t="s">
         <v>464</v>
       </c>
-      <c r="B54">
+      <c r="C54">
         <v>11</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E54" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>975</v>
+      </c>
+      <c r="B55" t="s">
         <v>465</v>
       </c>
-      <c r="B55">
+      <c r="C55">
         <v>15</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
+        <v>1049</v>
+      </c>
+      <c r="E55" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>976</v>
+      </c>
+      <c r="B56" t="s">
         <v>466</v>
       </c>
-      <c r="B56">
+      <c r="C56">
         <v>16</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D56" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="E56" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>977</v>
+      </c>
+      <c r="B57" t="s">
         <v>467</v>
       </c>
-      <c r="B57">
+      <c r="C57">
         <v>11</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E57" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>978</v>
+      </c>
+      <c r="B58" t="s">
         <v>468</v>
       </c>
-      <c r="B58">
+      <c r="C58">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D58" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="E58" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>979</v>
+      </c>
+      <c r="B59" t="s">
         <v>469</v>
       </c>
-      <c r="B59">
+      <c r="C59">
         <v>45</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="E59" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>980</v>
+      </c>
+      <c r="B60" t="s">
         <v>470</v>
       </c>
-      <c r="B60">
+      <c r="C60">
         <v>11</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D60" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E60" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>981</v>
+      </c>
+      <c r="B61" t="s">
         <v>471</v>
       </c>
-      <c r="B61">
+      <c r="C61">
         <v>58</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D61" s="1" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E61" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>982</v>
+      </c>
+      <c r="B62" t="s">
         <v>472</v>
       </c>
-      <c r="B62">
+      <c r="C62">
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D62" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E62" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>983</v>
+      </c>
+      <c r="B63" t="s">
         <v>473</v>
       </c>
-      <c r="B63">
+      <c r="C63">
         <v>56</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D63" s="1" t="s">
+        <v>1057</v>
+      </c>
+      <c r="E63" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>984</v>
+      </c>
+      <c r="B64" t="s">
         <v>474</v>
       </c>
-      <c r="B64">
+      <c r="C64">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D64" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="E64" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>985</v>
+      </c>
+      <c r="B65" t="s">
         <v>475</v>
       </c>
-      <c r="B65">
+      <c r="C65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D65" s="1" t="s">
+        <v>1059</v>
+      </c>
+      <c r="E65" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>986</v>
+      </c>
+      <c r="B66" t="s">
         <v>476</v>
       </c>
-      <c r="B66">
+      <c r="C66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D66" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="E66" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>987</v>
+      </c>
+      <c r="B67" t="s">
         <v>477</v>
       </c>
-      <c r="B67">
+      <c r="C67">
         <v>11</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D67" s="1" t="s">
+        <v>1061</v>
+      </c>
+      <c r="E67" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>988</v>
+      </c>
+      <c r="B68" t="s">
         <v>478</v>
       </c>
-      <c r="B68">
+      <c r="C68">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D68" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E68" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>989</v>
+      </c>
+      <c r="B69" t="s">
         <v>479</v>
       </c>
-      <c r="B69">
+      <c r="C69">
         <v>85</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D69" s="1" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E69" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>990</v>
+      </c>
+      <c r="B70" t="s">
         <v>480</v>
       </c>
-      <c r="B70">
+      <c r="C70">
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D70" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E70" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>991</v>
+      </c>
+      <c r="B71" t="s">
         <v>481</v>
       </c>
-      <c r="B71">
+      <c r="C71">
         <v>11</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D71" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="E71" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>992</v>
+      </c>
+      <c r="B72" t="s">
         <v>482</v>
       </c>
-      <c r="B72">
+      <c r="C72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D72" s="1" t="s">
+        <v>1066</v>
+      </c>
+      <c r="E72" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>993</v>
+      </c>
+      <c r="B73" t="s">
         <v>483</v>
       </c>
-      <c r="B73">
+      <c r="C73">
         <v>6</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D73" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E73" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>994</v>
+      </c>
+      <c r="B74" t="s">
         <v>484</v>
       </c>
-      <c r="B74">
+      <c r="C74">
         <v>7</v>
       </c>
+      <c r="D74" s="1" t="s">
+        <v>1068</v>
+      </c>
+      <c r="E74" t="s">
+        <v>507</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{4AC549A9-421E-4582-94DC-8B68B44A679A}"/>
+    <hyperlink ref="D3:D74" r:id="rId2" display="https://euipo.europa.eu/ohimportal/nl/databases/ProductID0001" xr:uid="{B942FC27-FB03-4D75-B08D-05F374D32CE4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Kleine wijzigingen testdata en assertions
</commit_message>
<xml_diff>
--- a/test/testdata.xlsx
+++ b/test/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Blockathon_hyper42\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DCA278-406F-48F4-BF30-4E6AC9185B47}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A1DE594-556F-4D94-90E5-0482F9A29E9D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" activeTab="3" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" xr2:uid="{A8368FE9-5A84-4C05-BC24-FA3A00CF4C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Manufacturer" sheetId="1" r:id="rId1"/>
@@ -3600,7 +3600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3382E85-A5EE-423B-83A5-84997E0C5C39}">
   <dimension ref="A1:B324"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
@@ -6978,7 +6978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F13C3947-283C-45EE-B2FB-975473C10A44}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>